<commit_message>
add group func and cp data up
</commit_message>
<xml_diff>
--- a/_back/cp/15.xlsx
+++ b/_back/cp/15.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="122211" refMode="R1C1"/>
@@ -49,7 +49,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -68,6 +68,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -81,7 +87,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -111,6 +117,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -414,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O30"/>
+  <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="O1" activeCellId="4" sqref="A1:A1048576 F1:F1048576 I1:I1048576 J1:J1048576 O1:O1048576"/>
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1135,7 +1144,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A16" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B16" s="1">
         <v>0</v>
@@ -1180,7 +1189,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B17" s="1">
         <v>10</v>
       </c>
@@ -1203,7 +1212,7 @@
         <v>0</v>
       </c>
       <c r="I17" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J17" s="4">
         <v>7</v>
@@ -1220,8 +1229,11 @@
       <c r="N17" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="O17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B18" s="1">
         <v>0</v>
       </c>
@@ -1244,7 +1256,7 @@
         <v>0</v>
       </c>
       <c r="J18" s="4">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="K18" s="4">
         <v>3</v>
@@ -1258,10 +1270,13 @@
       <c r="N18" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="O18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B19" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C19" s="1">
         <v>3</v>
@@ -1275,6 +1290,9 @@
       <c r="F19" s="1">
         <v>0</v>
       </c>
+      <c r="G19" s="1">
+        <v>0</v>
+      </c>
       <c r="H19" s="1">
         <v>3</v>
       </c>
@@ -1282,7 +1300,7 @@
         <v>0</v>
       </c>
       <c r="L19" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M19" s="4">
         <v>1</v>
@@ -1290,19 +1308,34 @@
       <c r="N19" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="O19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.15">
       <c r="C20" s="1">
         <v>2</v>
       </c>
       <c r="D20" s="1">
         <v>1</v>
       </c>
+      <c r="E20" s="1">
+        <v>2</v>
+      </c>
       <c r="F20" s="1">
         <v>0</v>
       </c>
+      <c r="G20" s="1">
+        <v>0</v>
+      </c>
       <c r="H20" s="1">
         <v>0</v>
+      </c>
+      <c r="K20" s="4">
+        <v>2</v>
+      </c>
+      <c r="L20" s="4">
+        <v>1</v>
       </c>
       <c r="M20" s="4">
         <v>0</v>
@@ -1311,7 +1344,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.15">
       <c r="C21" s="1">
         <v>0</v>
       </c>
@@ -1321,6 +1354,9 @@
       <c r="F21" s="1">
         <v>2</v>
       </c>
+      <c r="G21" s="1">
+        <v>0</v>
+      </c>
       <c r="H21" s="1">
         <v>2</v>
       </c>
@@ -1331,9 +1367,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.15">
       <c r="C22" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D22" s="1">
         <v>4</v>
@@ -1348,10 +1384,13 @@
         <v>1</v>
       </c>
       <c r="N22" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="D23" s="1">
+        <v>2</v>
+      </c>
       <c r="F23" s="1">
         <v>2</v>
       </c>
@@ -1361,8 +1400,11 @@
       <c r="M23" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="N23" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.15">
       <c r="F24" s="1">
         <v>2</v>
       </c>
@@ -1372,8 +1414,11 @@
       <c r="M24" s="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.15">
+      <c r="N24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.15">
       <c r="F25" s="1">
         <v>4</v>
       </c>
@@ -1384,7 +1429,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:15" x14ac:dyDescent="0.15">
       <c r="F26" s="1">
         <v>0</v>
       </c>
@@ -1395,7 +1440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="27" spans="2:15" x14ac:dyDescent="0.15">
       <c r="F27" s="1">
         <v>0</v>
       </c>
@@ -1406,7 +1451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.15">
       <c r="F28" s="1">
         <v>0</v>
       </c>
@@ -1417,20 +1462,31 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.15">
+    <row r="29" spans="2:15" x14ac:dyDescent="0.15">
       <c r="F29" s="1">
         <v>0</v>
       </c>
       <c r="H29" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M29" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.15">
       <c r="F30" s="1">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="H30" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.15">
+      <c r="F31" s="1">
+        <v>0</v>
+      </c>
+      <c r="H31" s="1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1441,10 +1497,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A75:AD107"/>
+  <dimension ref="A75:AD108"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="W102" sqref="W102"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="M104" sqref="M104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2993,7 +3049,7 @@
         <v>0</v>
       </c>
       <c r="N97" s="5">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="O97" s="6">
         <v>0</v>
@@ -3063,7 +3119,7 @@
       </c>
       <c r="L98" s="4"/>
       <c r="M98" s="5">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="N98" s="6">
         <v>4</v>
@@ -3072,7 +3128,7 @@
         <v>0</v>
       </c>
       <c r="P98" s="5">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="Q98" s="6">
         <v>1</v>
@@ -3086,12 +3142,8 @@
       <c r="U98" s="6">
         <v>4</v>
       </c>
-      <c r="V98" s="5">
-        <v>6</v>
-      </c>
-      <c r="W98" s="5">
-        <v>6</v>
-      </c>
+      <c r="V98" s="5"/>
+      <c r="W98" s="5"/>
       <c r="Z98" s="1">
         <v>0</v>
       </c>
@@ -3149,6 +3201,7 @@
       <c r="Q99" s="6">
         <v>1</v>
       </c>
+      <c r="R99" s="5"/>
       <c r="S99" s="6">
         <v>0</v>
       </c>
@@ -3212,7 +3265,7 @@
         <v>6</v>
       </c>
       <c r="L100" s="4"/>
-      <c r="M100" s="5">
+      <c r="M100" s="6">
         <v>4</v>
       </c>
       <c r="N100" s="6">
@@ -3227,6 +3280,7 @@
       <c r="Q100" s="6">
         <v>0</v>
       </c>
+      <c r="R100" s="5"/>
       <c r="S100" s="3">
         <v>0</v>
       </c>
@@ -3238,6 +3292,9 @@
       </c>
       <c r="V100" s="3">
         <v>3</v>
+      </c>
+      <c r="W100" s="3">
+        <v>4</v>
       </c>
       <c r="Z100" s="1">
         <v>0</v>
@@ -3290,15 +3347,16 @@
       <c r="N101" s="6">
         <v>2</v>
       </c>
-      <c r="O101" s="5">
-        <v>3</v>
+      <c r="O101" s="6">
+        <v>4</v>
       </c>
       <c r="P101" s="6">
         <v>0</v>
       </c>
-      <c r="Q101" s="5">
-        <v>3</v>
-      </c>
+      <c r="Q101" s="6">
+        <v>3</v>
+      </c>
+      <c r="R101" s="5"/>
       <c r="S101" s="3">
         <v>0</v>
       </c>
@@ -3308,8 +3366,11 @@
       <c r="U101" s="3">
         <v>2</v>
       </c>
-      <c r="V101" s="2">
-        <v>3</v>
+      <c r="V101" s="3">
+        <v>3</v>
+      </c>
+      <c r="W101" s="3">
+        <v>4</v>
       </c>
       <c r="Z101" s="1">
         <v>0</v>
@@ -3363,11 +3424,12 @@
         <v>0</v>
       </c>
       <c r="P102" s="5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="Q102" s="6">
         <v>1</v>
       </c>
+      <c r="R102" s="5"/>
       <c r="S102" s="3">
         <v>0</v>
       </c>
@@ -3425,26 +3487,33 @@
       <c r="M103" s="6">
         <v>0</v>
       </c>
-      <c r="N103" s="5">
-        <v>1</v>
-      </c>
-      <c r="O103" s="5">
-        <v>1</v>
-      </c>
-      <c r="P103" s="5">
+      <c r="N103" s="6">
+        <v>1</v>
+      </c>
+      <c r="O103" s="11">
+        <v>3</v>
+      </c>
+      <c r="P103" s="6">
         <v>1</v>
       </c>
       <c r="Q103" s="6">
         <v>0</v>
       </c>
+      <c r="R103" s="5"/>
       <c r="S103" s="3">
         <v>0</v>
       </c>
       <c r="T103" s="3">
         <v>0</v>
       </c>
-      <c r="U103" s="2">
-        <v>1</v>
+      <c r="U103" s="3">
+        <v>1</v>
+      </c>
+      <c r="V103" s="3">
+        <v>1</v>
+      </c>
+      <c r="W103" s="3">
+        <v>3</v>
       </c>
       <c r="Z103" s="1">
         <v>0</v>
@@ -3489,22 +3558,29 @@
       </c>
       <c r="L104" s="4"/>
       <c r="M104" s="5">
-        <v>0</v>
-      </c>
-      <c r="N104" s="5">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="N104" s="6">
+        <v>1</v>
       </c>
       <c r="O104" s="5">
-        <v>0</v>
-      </c>
-      <c r="P104" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q104" s="5">
-        <v>0</v>
-      </c>
-      <c r="S104" s="2">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="P104" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q104" s="6">
+        <v>1</v>
+      </c>
+      <c r="R104" s="5"/>
+      <c r="S104" s="3">
+        <v>0</v>
+      </c>
+      <c r="T104" s="3">
+        <v>1</v>
+      </c>
+      <c r="U104" s="3">
+        <v>1</v>
       </c>
       <c r="Z104" s="1">
         <v>0</v>
@@ -3520,35 +3596,202 @@
       </c>
     </row>
     <row r="105" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A105" s="1">
+        <v>4</v>
+      </c>
+      <c r="B105" s="1">
+        <v>1</v>
+      </c>
+      <c r="C105" s="1">
+        <v>1</v>
+      </c>
+      <c r="D105" s="1">
+        <v>0</v>
+      </c>
+      <c r="E105" s="1">
+        <v>3</v>
+      </c>
       <c r="G105" s="1">
         <v>0</v>
       </c>
+      <c r="H105" s="1">
+        <v>1</v>
+      </c>
+      <c r="I105" s="1">
+        <v>1</v>
+      </c>
       <c r="J105" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="K105" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L105" s="4"/>
-      <c r="M105" s="5"/>
-      <c r="N105" s="5"/>
-      <c r="O105" s="5"/>
-      <c r="P105" s="5"/>
-      <c r="Q105" s="5"/>
+      <c r="M105" s="5">
+        <v>2</v>
+      </c>
+      <c r="N105" s="5">
+        <v>2</v>
+      </c>
+      <c r="O105" s="6">
+        <v>0</v>
+      </c>
+      <c r="P105" s="5">
+        <v>2</v>
+      </c>
+      <c r="Q105" s="6">
+        <v>0</v>
+      </c>
+      <c r="R105" s="5"/>
+      <c r="S105" s="3">
+        <v>0</v>
+      </c>
+      <c r="T105" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z105" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA105" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB105" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC105" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="106" spans="1:30" x14ac:dyDescent="0.15">
-      <c r="M106" s="5"/>
-      <c r="N106" s="5"/>
-      <c r="O106" s="5"/>
-      <c r="P106" s="5"/>
-      <c r="Q106" s="5"/>
+      <c r="A106" s="1">
+        <v>0</v>
+      </c>
+      <c r="B106" s="1">
+        <v>1</v>
+      </c>
+      <c r="C106" s="1">
+        <v>4</v>
+      </c>
+      <c r="D106" s="1">
+        <v>1</v>
+      </c>
+      <c r="E106" s="1">
+        <v>0</v>
+      </c>
+      <c r="G106" s="1">
+        <v>0</v>
+      </c>
+      <c r="H106" s="1">
+        <v>0</v>
+      </c>
+      <c r="I106" s="1">
+        <v>1</v>
+      </c>
+      <c r="J106" s="1">
+        <v>1</v>
+      </c>
+      <c r="K106" s="1">
+        <v>4</v>
+      </c>
+      <c r="M106" s="11">
+        <v>0</v>
+      </c>
+      <c r="N106" s="11">
+        <v>0</v>
+      </c>
+      <c r="O106" s="5">
+        <v>1</v>
+      </c>
+      <c r="P106" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q106" s="11">
+        <v>0</v>
+      </c>
+      <c r="R106" s="5"/>
+      <c r="S106" s="3">
+        <v>0</v>
+      </c>
+      <c r="T106" s="3">
+        <v>0</v>
+      </c>
+      <c r="U106" s="3">
+        <v>0</v>
+      </c>
+      <c r="V106" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z106" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA106" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB106" s="1">
+        <v>4</v>
+      </c>
     </row>
     <row r="107" spans="1:30" x14ac:dyDescent="0.15">
-      <c r="M107" s="5"/>
-      <c r="N107" s="5"/>
-      <c r="O107" s="5"/>
-      <c r="P107" s="5"/>
-      <c r="Q107" s="5"/>
+      <c r="A107" s="1">
+        <v>3</v>
+      </c>
+      <c r="B107" s="1">
+        <v>0</v>
+      </c>
+      <c r="C107" s="1">
+        <v>0</v>
+      </c>
+      <c r="D107" s="1">
+        <v>0</v>
+      </c>
+      <c r="E107" s="1">
+        <v>0</v>
+      </c>
+      <c r="G107" s="1">
+        <v>0</v>
+      </c>
+      <c r="H107" s="1">
+        <v>0</v>
+      </c>
+      <c r="I107" s="1">
+        <v>0</v>
+      </c>
+      <c r="J107" s="1">
+        <v>0</v>
+      </c>
+      <c r="K107" s="1">
+        <v>3</v>
+      </c>
+      <c r="M107" s="5">
+        <v>0</v>
+      </c>
+      <c r="N107" s="5">
+        <v>0</v>
+      </c>
+      <c r="O107" s="5">
+        <v>0</v>
+      </c>
+      <c r="P107" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q107" s="5">
+        <v>0</v>
+      </c>
+      <c r="R107" s="5"/>
+      <c r="Z107" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA107" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="108" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="M108" s="5"/>
+      <c r="N108" s="5"/>
+      <c r="O108" s="5"/>
+      <c r="P108" s="5"/>
+      <c r="Q108" s="5"/>
+      <c r="R108" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -3559,10 +3802,275 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A76:U105"/>
+  <dimension ref="A90:K107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="M114" sqref="M114"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="J113" sqref="J113"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="32" width="5.625" style="8" customWidth="1"/>
+    <col min="33" max="16384" width="9" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A90" s="7">
+        <v>2</v>
+      </c>
+      <c r="C90" s="9">
+        <v>1</v>
+      </c>
+      <c r="H90" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A91" s="9">
+        <v>1</v>
+      </c>
+      <c r="B91" s="9">
+        <v>1</v>
+      </c>
+      <c r="C91" s="9">
+        <v>1</v>
+      </c>
+      <c r="D91" s="9">
+        <v>1</v>
+      </c>
+      <c r="E91" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A92" s="9">
+        <v>1</v>
+      </c>
+      <c r="B92" s="7">
+        <v>3</v>
+      </c>
+      <c r="E92" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A93" s="7">
+        <v>2</v>
+      </c>
+      <c r="B93" s="9">
+        <v>1</v>
+      </c>
+      <c r="H93" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A94" s="7">
+        <v>2</v>
+      </c>
+      <c r="B94" s="9">
+        <v>1</v>
+      </c>
+      <c r="C94" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A95" s="7">
+        <v>2</v>
+      </c>
+      <c r="D95" s="9">
+        <v>1</v>
+      </c>
+      <c r="G95" s="9">
+        <v>1</v>
+      </c>
+      <c r="I95" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A96" s="9">
+        <v>1</v>
+      </c>
+      <c r="B96" s="9">
+        <v>1</v>
+      </c>
+      <c r="C96" s="7">
+        <v>2</v>
+      </c>
+      <c r="D96" s="9">
+        <v>1</v>
+      </c>
+      <c r="F96" s="10"/>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A97" s="7">
+        <v>2</v>
+      </c>
+      <c r="B97" s="9">
+        <v>1</v>
+      </c>
+      <c r="C97" s="9">
+        <v>1</v>
+      </c>
+      <c r="H97" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A98" s="7">
+        <v>3</v>
+      </c>
+      <c r="C98" s="9">
+        <v>1</v>
+      </c>
+      <c r="H98" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A99" s="9">
+        <v>1</v>
+      </c>
+      <c r="B99" s="9">
+        <v>1</v>
+      </c>
+      <c r="C99" s="9">
+        <v>1</v>
+      </c>
+      <c r="D99" s="9">
+        <v>1</v>
+      </c>
+      <c r="E99" s="9">
+        <v>1</v>
+      </c>
+      <c r="G99" s="10"/>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A100" s="7">
+        <v>2</v>
+      </c>
+      <c r="B100" s="9">
+        <v>1</v>
+      </c>
+      <c r="D100" s="9">
+        <v>1</v>
+      </c>
+      <c r="G100" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A101" s="7">
+        <v>3</v>
+      </c>
+      <c r="B101" s="9">
+        <v>1</v>
+      </c>
+      <c r="C101" s="10"/>
+      <c r="D101" s="10"/>
+      <c r="E101" s="9">
+        <v>1</v>
+      </c>
+      <c r="F101" s="10"/>
+      <c r="G101" s="10"/>
+      <c r="H101" s="10"/>
+      <c r="I101" s="10"/>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A102" s="7">
+        <v>2</v>
+      </c>
+      <c r="B102" s="10"/>
+      <c r="C102" s="7">
+        <v>2</v>
+      </c>
+      <c r="D102" s="10"/>
+      <c r="E102" s="10"/>
+      <c r="G102" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A103" s="7">
+        <v>3</v>
+      </c>
+      <c r="B103" s="10"/>
+      <c r="C103" s="10"/>
+      <c r="D103" s="10"/>
+      <c r="E103" s="9">
+        <v>1</v>
+      </c>
+      <c r="G103" s="10"/>
+      <c r="K103" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A104" s="7">
+        <v>2</v>
+      </c>
+      <c r="B104" s="9">
+        <v>1</v>
+      </c>
+      <c r="C104" s="9">
+        <v>1</v>
+      </c>
+      <c r="D104" s="9">
+        <v>1</v>
+      </c>
+      <c r="E104" s="10"/>
+      <c r="F104" s="10"/>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A105" s="9">
+        <v>1</v>
+      </c>
+      <c r="B105" s="7">
+        <v>2</v>
+      </c>
+      <c r="C105" s="10"/>
+      <c r="D105" s="9">
+        <v>1</v>
+      </c>
+      <c r="E105" s="9">
+        <v>1</v>
+      </c>
+      <c r="G105" s="10"/>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A106" s="7">
+        <v>2</v>
+      </c>
+      <c r="B106" s="7">
+        <v>2</v>
+      </c>
+      <c r="D106" s="10"/>
+      <c r="E106" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A107" s="7">
+        <v>4</v>
+      </c>
+      <c r="D107" s="9">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A76:U107"/>
+  <sheetViews>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="E112" sqref="E112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4254,243 +4762,122 @@
       <c r="A105" s="1">
         <v>1</v>
       </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A90:K105"/>
-  <sheetViews>
-    <sheetView topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="H113" sqref="H113"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="32" width="5.625" style="8" customWidth="1"/>
-    <col min="33" max="16384" width="9" style="8"/>
-  </cols>
-  <sheetData>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A90" s="7">
-        <v>2</v>
-      </c>
-      <c r="C90" s="9">
-        <v>1</v>
-      </c>
-      <c r="H90" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A91" s="9">
-        <v>1</v>
-      </c>
-      <c r="B91" s="9">
-        <v>1</v>
-      </c>
-      <c r="C91" s="9">
-        <v>1</v>
-      </c>
-      <c r="D91" s="9">
-        <v>1</v>
-      </c>
-      <c r="E91" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A92" s="9">
-        <v>1</v>
-      </c>
-      <c r="B92" s="7">
-        <v>3</v>
-      </c>
-      <c r="E92" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A93" s="7">
-        <v>2</v>
-      </c>
-      <c r="B93" s="9">
-        <v>1</v>
-      </c>
-      <c r="H93" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A94" s="7">
-        <v>2</v>
-      </c>
-      <c r="B94" s="9">
-        <v>1</v>
-      </c>
-      <c r="C94" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A95" s="7">
-        <v>2</v>
-      </c>
-      <c r="D95" s="9">
-        <v>1</v>
-      </c>
-      <c r="G95" s="9">
-        <v>1</v>
-      </c>
-      <c r="I95" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A96" s="9">
-        <v>1</v>
-      </c>
-      <c r="B96" s="9">
-        <v>1</v>
-      </c>
-      <c r="C96" s="7">
-        <v>2</v>
-      </c>
-      <c r="D96" s="9">
-        <v>1</v>
-      </c>
-      <c r="F96" s="10"/>
-    </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A97" s="7">
-        <v>2</v>
-      </c>
-      <c r="B97" s="9">
-        <v>1</v>
-      </c>
-      <c r="C97" s="9">
-        <v>1</v>
-      </c>
-      <c r="H97" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A98" s="7">
-        <v>3</v>
-      </c>
-      <c r="C98" s="9">
-        <v>1</v>
-      </c>
-      <c r="H98" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A99" s="9">
-        <v>1</v>
-      </c>
-      <c r="B99" s="9">
-        <v>1</v>
-      </c>
-      <c r="C99" s="9">
-        <v>1</v>
-      </c>
-      <c r="D99" s="9">
-        <v>1</v>
-      </c>
-      <c r="E99" s="9">
-        <v>1</v>
-      </c>
-      <c r="G99" s="10"/>
-    </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A100" s="7">
-        <v>2</v>
-      </c>
-      <c r="B100" s="9">
-        <v>1</v>
-      </c>
-      <c r="D100" s="9">
-        <v>1</v>
-      </c>
-      <c r="G100" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A101" s="7">
-        <v>3</v>
-      </c>
-      <c r="B101" s="9">
-        <v>1</v>
-      </c>
-      <c r="C101" s="10"/>
-      <c r="D101" s="10"/>
-      <c r="E101" s="9">
-        <v>1</v>
-      </c>
-      <c r="F101" s="10"/>
-      <c r="G101" s="10"/>
-      <c r="H101" s="10"/>
-      <c r="I101" s="10"/>
-    </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A102" s="7">
-        <v>2</v>
-      </c>
-      <c r="B102" s="10"/>
-      <c r="C102" s="7">
-        <v>2</v>
-      </c>
-      <c r="D102" s="10"/>
-      <c r="E102" s="10"/>
-      <c r="G102" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A103" s="7">
-        <v>3</v>
-      </c>
-      <c r="B103" s="10"/>
-      <c r="C103" s="10"/>
-      <c r="D103" s="10"/>
-      <c r="E103" s="9">
-        <v>1</v>
-      </c>
-      <c r="G103" s="10"/>
-      <c r="K103" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A104" s="7">
-        <v>2</v>
-      </c>
-      <c r="B104" s="9">
-        <v>1</v>
-      </c>
-      <c r="C104" s="9">
-        <v>1</v>
-      </c>
-      <c r="D104" s="9">
-        <v>1</v>
-      </c>
-      <c r="E104" s="10"/>
-      <c r="F104" s="10"/>
-    </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A105" s="9">
-        <v>1</v>
-      </c>
-      <c r="C105" s="10"/>
-      <c r="D105" s="10"/>
-      <c r="G105" s="9">
+      <c r="B105" s="1">
+        <v>2</v>
+      </c>
+      <c r="C105" s="1">
+        <v>2</v>
+      </c>
+      <c r="H105" s="1">
+        <v>1</v>
+      </c>
+      <c r="I105" s="1">
+        <v>1</v>
+      </c>
+      <c r="J105" s="1">
+        <v>0</v>
+      </c>
+      <c r="K105" s="1">
+        <v>2</v>
+      </c>
+      <c r="L105" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q105" s="1">
+        <v>0</v>
+      </c>
+      <c r="R105" s="1">
+        <v>1</v>
+      </c>
+      <c r="S105" s="1">
+        <v>3</v>
+      </c>
+      <c r="T105" s="1">
+        <v>3</v>
+      </c>
+      <c r="U105" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="106" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A106" s="1">
+        <v>2</v>
+      </c>
+      <c r="B106" s="1">
+        <v>3</v>
+      </c>
+      <c r="C106" s="1">
+        <v>0</v>
+      </c>
+      <c r="H106" s="1">
+        <v>0</v>
+      </c>
+      <c r="I106" s="1">
+        <v>1</v>
+      </c>
+      <c r="J106" s="1">
+        <v>2</v>
+      </c>
+      <c r="K106" s="1">
+        <v>0</v>
+      </c>
+      <c r="L106" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q106" s="1">
+        <v>0</v>
+      </c>
+      <c r="R106" s="1">
+        <v>0</v>
+      </c>
+      <c r="S106" s="1">
+        <v>1</v>
+      </c>
+      <c r="T106" s="1">
+        <v>1</v>
+      </c>
+      <c r="U106" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="107" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A107" s="1">
+        <v>4</v>
+      </c>
+      <c r="B107" s="1">
+        <v>1</v>
+      </c>
+      <c r="C107" s="1">
+        <v>0</v>
+      </c>
+      <c r="H107" s="1">
+        <v>1</v>
+      </c>
+      <c r="I107" s="1">
+        <v>1</v>
+      </c>
+      <c r="J107" s="1">
+        <v>1</v>
+      </c>
+      <c r="K107" s="1">
+        <v>1</v>
+      </c>
+      <c r="L107" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q107" s="1">
+        <v>0</v>
+      </c>
+      <c r="R107" s="1">
+        <v>0</v>
+      </c>
+      <c r="S107" s="1">
+        <v>0</v>
+      </c>
+      <c r="T107" s="1">
+        <v>1</v>
+      </c>
+      <c r="U107" s="1">
         <v>1</v>
       </c>
     </row>
@@ -4502,10 +4889,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A91:AK105"/>
+  <dimension ref="A91:AK108"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="E105" sqref="E105:F105"/>
+    <sheetView topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="K117" sqref="K117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4514,7 +4901,7 @@
     <col min="11" max="37" width="5.625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A91" s="9">
         <v>1</v>
       </c>
@@ -4543,7 +4930,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A92" s="9">
         <v>1</v>
       </c>
@@ -4574,8 +4961,17 @@
       <c r="R92" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="V92" s="1">
+        <v>2</v>
+      </c>
+      <c r="W92" s="1">
+        <v>1</v>
+      </c>
+      <c r="X92" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A93" s="7">
         <v>2</v>
       </c>
@@ -4603,8 +4999,17 @@
       <c r="R93" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="V93" s="1">
+        <v>3</v>
+      </c>
+      <c r="W93" s="1">
+        <v>1</v>
+      </c>
+      <c r="X93" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A94" s="9">
         <v>1</v>
       </c>
@@ -4635,8 +5040,17 @@
       <c r="R94" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="V94" s="1">
+        <v>3</v>
+      </c>
+      <c r="W94" s="1">
+        <v>1</v>
+      </c>
+      <c r="X94" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:24" x14ac:dyDescent="0.15">
       <c r="B95" s="9">
         <v>1</v>
       </c>
@@ -4664,8 +5078,17 @@
       <c r="R95" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="V95" s="1">
+        <v>3</v>
+      </c>
+      <c r="W95" s="1">
+        <v>1</v>
+      </c>
+      <c r="X95" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:24" x14ac:dyDescent="0.15">
       <c r="C96" s="9">
         <v>1</v>
       </c>
@@ -4696,8 +5119,17 @@
       <c r="R96" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="V96" s="1">
+        <v>3</v>
+      </c>
+      <c r="W96" s="1">
+        <v>0</v>
+      </c>
+      <c r="X96" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A97" s="9">
         <v>1</v>
       </c>
@@ -4726,8 +5158,17 @@
       <c r="R97" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="V97" s="1">
+        <v>2</v>
+      </c>
+      <c r="W97" s="1">
+        <v>1</v>
+      </c>
+      <c r="X97" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A98" s="9">
         <v>1</v>
       </c>
@@ -4758,8 +5199,17 @@
       <c r="R98" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="V98" s="1">
+        <v>4</v>
+      </c>
+      <c r="W98" s="1">
+        <v>0</v>
+      </c>
+      <c r="X98" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:24" x14ac:dyDescent="0.15">
       <c r="B99" s="9">
         <v>1</v>
       </c>
@@ -4790,8 +5240,17 @@
       <c r="R99" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="V99" s="1">
+        <v>2</v>
+      </c>
+      <c r="W99" s="1">
+        <v>3</v>
+      </c>
+      <c r="X99" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A100" s="9">
         <v>1</v>
       </c>
@@ -4822,8 +5281,17 @@
       <c r="R100" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="V100" s="1">
+        <v>2</v>
+      </c>
+      <c r="W100" s="1">
+        <v>3</v>
+      </c>
+      <c r="X100" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:24" x14ac:dyDescent="0.15">
       <c r="B101" s="9">
         <v>1</v>
       </c>
@@ -4854,8 +5322,17 @@
       <c r="R101" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="V101" s="1">
+        <v>3</v>
+      </c>
+      <c r="W101" s="1">
+        <v>1</v>
+      </c>
+      <c r="X101" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:24" x14ac:dyDescent="0.15">
       <c r="C102" s="9">
         <v>1</v>
       </c>
@@ -4886,8 +5363,17 @@
       <c r="R102" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="V102" s="1">
+        <v>2</v>
+      </c>
+      <c r="W102" s="1">
+        <v>3</v>
+      </c>
+      <c r="X102" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:24" x14ac:dyDescent="0.15">
       <c r="B103" s="9">
         <v>1</v>
       </c>
@@ -4918,8 +5404,17 @@
       <c r="R103" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="104" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="V103" s="1">
+        <v>3</v>
+      </c>
+      <c r="W103" s="1">
+        <v>2</v>
+      </c>
+      <c r="X103" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A104" s="9">
         <v>1</v>
       </c>
@@ -4950,26 +5445,143 @@
       <c r="R104" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="V104" s="1">
+        <v>2</v>
+      </c>
+      <c r="W104" s="1">
+        <v>3</v>
+      </c>
+      <c r="X104" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A105" s="9">
+        <v>1</v>
+      </c>
+      <c r="D105" s="9">
+        <v>1</v>
+      </c>
+      <c r="E105" s="7">
+        <v>2</v>
+      </c>
       <c r="G105" s="9">
         <v>1</v>
       </c>
       <c r="N105" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O105" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="P105" s="1">
         <v>5</v>
       </c>
       <c r="Q105" s="1">
+        <v>5</v>
+      </c>
+      <c r="R105" s="1">
+        <v>7</v>
+      </c>
+      <c r="V105" s="1">
+        <v>2</v>
+      </c>
+      <c r="W105" s="1">
+        <v>2</v>
+      </c>
+      <c r="X105" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A106" s="10"/>
+      <c r="B106" s="9">
+        <v>1</v>
+      </c>
+      <c r="D106" s="9">
+        <v>1</v>
+      </c>
+      <c r="E106" s="9">
+        <v>1</v>
+      </c>
+      <c r="F106" s="10"/>
+      <c r="G106" s="9">
+        <v>1</v>
+      </c>
+      <c r="H106" s="9">
+        <v>1</v>
+      </c>
+      <c r="I106" s="10"/>
+      <c r="J106" s="10"/>
+      <c r="N106" s="1">
+        <v>2</v>
+      </c>
+      <c r="O106" s="1">
+        <v>4</v>
+      </c>
+      <c r="P106" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q106" s="1">
+        <v>7</v>
+      </c>
+      <c r="R106" s="1">
+        <v>8</v>
+      </c>
+      <c r="V106" s="1">
+        <v>3</v>
+      </c>
+      <c r="W106" s="1">
+        <v>2</v>
+      </c>
+      <c r="X106" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="B107" s="10"/>
+      <c r="D107" s="9">
+        <v>1</v>
+      </c>
+      <c r="E107" s="9">
+        <v>1</v>
+      </c>
+      <c r="F107" s="9">
+        <v>1</v>
+      </c>
+      <c r="G107" s="9">
+        <v>1</v>
+      </c>
+      <c r="H107" s="9">
+        <v>1</v>
+      </c>
+      <c r="N107" s="1">
+        <v>4</v>
+      </c>
+      <c r="O107" s="1">
+        <v>5</v>
+      </c>
+      <c r="P107" s="1">
         <v>6</v>
       </c>
-      <c r="R105" s="1">
-        <v>9</v>
-      </c>
+      <c r="Q107" s="1">
+        <v>7</v>
+      </c>
+      <c r="R107" s="1">
+        <v>8</v>
+      </c>
+      <c r="V107" s="1">
+        <v>4</v>
+      </c>
+      <c r="W107" s="1">
+        <v>1</v>
+      </c>
+      <c r="X107" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="E108" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>